<commit_message>
Tested Model with Operation Start on Dec 1, 2018
Minor changes to rules were made during debugging to better match the Model outputs with the IGD Calc. In addition, many hard input constants or DateTimes were changed to be referenced to slots on objects to ease future editing.
An R Script was developed to automate the comparison between the IGD Calc. and the RiverWare Model. Instructions on how to complete the testing have been uploaded as well.
</commit_message>
<xml_diff>
--- a/DMI Sheet/flowcalc.xlsx
+++ b/DMI Sheet/flowcalc.xlsx
@@ -6027,9 +6027,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W602"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A585" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C606" sqref="C606"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q261" sqref="Q261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23079,7 +23079,7 @@
         <v>95.6</v>
       </c>
       <c r="P246">
-        <v>68.473333333336697</v>
+        <v>73</v>
       </c>
       <c r="Q246">
         <v>0</v>

</xml_diff>

<commit_message>
Minor updates to functions and rules in the merged model
Changed the Op Percentile slots from scalar to series so it can account for different values from year to year

Added in new function to handle setting the correct water year that is used for projecting accretion values ~ WhichOpYear ( )

Edited the script to clear slots set by initialization rules that cause errors when testing different operation start dates

Updated the UKL and Williamson Inflow Projection Rules to work on dates prior to Oct 1, 2018

Debugged the updated model to make sure these changes operated as intended

Currently the model is having issues running with an Operation Start Date before Oct 1, 2018
For other purposes the operation start date will need to be set after this until corrections are made
</commit_message>
<xml_diff>
--- a/DMI Sheet/flowcalc.xlsx
+++ b/DMI Sheet/flowcalc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>IGD.Outflow (cfs)</t>
   </si>
@@ -3148,7 +3148,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3167,6 +3167,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2579">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -6028,8 +6031,8 @@
   <dimension ref="A1:W602"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A359" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I393" sqref="I393"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6143,6 +6146,9 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
+      <c r="J3" s="6">
+        <v>957</v>
+      </c>
       <c r="L3">
         <v>509</v>
       </c>
@@ -6156,6 +6162,9 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
+      <c r="J4" s="6">
+        <v>991</v>
+      </c>
       <c r="L4">
         <v>509</v>
       </c>
@@ -6169,6 +6178,9 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
+      <c r="J5" s="6">
+        <v>959</v>
+      </c>
       <c r="L5">
         <v>507</v>
       </c>
@@ -6182,6 +6194,9 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
+      <c r="J6" s="6">
+        <v>965</v>
+      </c>
       <c r="L6">
         <v>507</v>
       </c>
@@ -6195,6 +6210,9 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
+      <c r="J7" s="6">
+        <v>964</v>
+      </c>
       <c r="L7">
         <v>508</v>
       </c>
@@ -6208,6 +6226,9 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
+      <c r="J8" s="6">
+        <v>958</v>
+      </c>
       <c r="L8">
         <v>567</v>
       </c>
@@ -8009,7 +8030,9 @@
       <c r="F34" s="7">
         <v>0</v>
       </c>
-      <c r="G34" s="5"/>
+      <c r="G34" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="H34" s="3">
         <v>550</v>
       </c>
@@ -8078,7 +8101,9 @@
       <c r="F35" s="7">
         <v>0</v>
       </c>
-      <c r="G35" s="5"/>
+      <c r="G35" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="H35" s="3">
         <v>500</v>
       </c>
@@ -8644,7 +8669,9 @@
       <c r="F43" s="7">
         <v>0</v>
       </c>
-      <c r="G43" s="5"/>
+      <c r="G43" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="H43" s="3">
         <v>500</v>
       </c>
@@ -20996,7 +21023,9 @@
       <c r="F217" s="7">
         <v>-60</v>
       </c>
-      <c r="G217" s="5"/>
+      <c r="G217" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="H217" s="3">
         <v>260</v>
       </c>
@@ -21065,7 +21094,9 @@
       <c r="F218" s="7">
         <v>-60</v>
       </c>
-      <c r="G218" s="5"/>
+      <c r="G218" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="H218" s="3">
         <v>260</v>
       </c>

</xml_diff>